<commit_message>
acceuil liste annonce all
</commit_message>
<xml_diff>
--- a/tools/TODO.xlsx
+++ b/tools/TODO.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="83">
   <si>
     <t>créer des data de cv remplis</t>
   </si>
@@ -223,13 +223,752 @@
   </si>
   <si>
     <t>selection entretien -&gt; voir plus</t>
+  </si>
+  <si>
+    <t>MIOVA NY VUE v_liste_cv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOUVELLE VUE </t>
+  </si>
+  <si>
+    <t>-- recrutement dept</t>
+  </si>
+  <si>
+    <r>
+      <t>CREATE OR REPLACE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VIEW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFA6E22E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>v_recrutement_dept</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>AS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>SELECT</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>*</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> recrutements recru </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>LEFT JOIN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> services s </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id_service</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>recru</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id_service_recrutement</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>LEFT JOIN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> departements dept </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id_dept_service</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>dept</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id_dept</t>
+    </r>
+  </si>
+  <si>
+    <t>);</t>
+  </si>
+  <si>
+    <t>-- user departement</t>
+  </si>
+  <si>
+    <r>
+      <t>CREATE OR REPLACE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VIEW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFA6E22E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>v_user_dept</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>AS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> users u </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>LEFT JOIN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> user_departements u_dept </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>u_dept</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id_user_user_dept</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>u</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id_user</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>LEFT JOIN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> departements dept </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>ON</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>u_dept</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id_dept_user_dept</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>=</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>dept</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFAE81FF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>id_dept</t>
+    </r>
+  </si>
+  <si>
+    <t>-- service departement</t>
+  </si>
+  <si>
+    <r>
+      <t>CREATE OR REPLACE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>VIEW</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFA6E22E"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>v_service_dept</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF92672"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>AS</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> (</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>FROM</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFF8F8F2"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> services s </t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,13 +976,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFF8F8F2"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF88846F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFF92672"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFA6E22E"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFAE81FF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF272822"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -258,12 +1033,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,10 +1585,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -809,7 +1596,8 @@
     <col min="1" max="1" width="26.33203125" customWidth="1"/>
     <col min="2" max="2" width="31" customWidth="1"/>
     <col min="3" max="3" width="26.77734375" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25.44140625" customWidth="1"/>
+    <col min="7" max="7" width="35.77734375" customWidth="1"/>
     <col min="8" max="8" width="19.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -873,6 +1661,9 @@
       <c r="C5" t="s">
         <v>40</v>
       </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
       <c r="H5" t="s">
         <v>64</v>
       </c>
@@ -887,6 +1678,9 @@
       <c r="C6" t="s">
         <v>41</v>
       </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
       <c r="H6" t="s">
         <v>64</v>
       </c>
@@ -904,6 +1698,9 @@
       <c r="D7" t="s">
         <v>38</v>
       </c>
+      <c r="G7">
+        <v>100</v>
+      </c>
       <c r="H7" t="s">
         <v>64</v>
       </c>
@@ -1041,7 +1838,124 @@
         <v>61</v>
       </c>
     </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A31" s="6"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" s="6"/>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TODO maj 3eme miaritory
</commit_message>
<xml_diff>
--- a/tools/TODO.xlsx
+++ b/tools/TODO.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5928" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="2eme fieretatory" sheetId="2" r:id="rId2"/>
+    <sheet name="3 eme fieretatory - contrat" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="96">
   <si>
     <t>créer des data de cv remplis</t>
   </si>
@@ -962,6 +963,45 @@
       </rPr>
       <t xml:space="preserve"> services s </t>
     </r>
+  </si>
+  <si>
+    <t>liste des entretiens</t>
+  </si>
+  <si>
+    <t>detail entretien</t>
+  </si>
+  <si>
+    <t>choix d'embauche</t>
+  </si>
+  <si>
+    <t>liste futur emp</t>
+  </si>
+  <si>
+    <t>creation contrat essai</t>
+  </si>
+  <si>
+    <t>resume contrat essai</t>
+  </si>
+  <si>
+    <t>liste contrat essai</t>
+  </si>
+  <si>
+    <t>detail contrat essai</t>
+  </si>
+  <si>
+    <t>chgt contrat - choix contrat</t>
+  </si>
+  <si>
+    <t>Taches</t>
+  </si>
+  <si>
+    <t>Qui</t>
+  </si>
+  <si>
+    <t>maj insertion besoin recrutement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ny avo </t>
   </si>
 </sst>
 </file>
@@ -1587,7 +1627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
@@ -1958,4 +1998,110 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
print PDF contrat esssai
</commit_message>
<xml_diff>
--- a/tools/TODO.xlsx
+++ b/tools/TODO.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="97">
   <si>
     <t>créer des data de cv remplis</t>
   </si>
@@ -2008,7 +2008,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2077,6 +2077,9 @@
       <c r="B7" t="s">
         <v>64</v>
       </c>
+      <c r="C7" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
@@ -2084,6 +2087,9 @@
       </c>
       <c r="B8" t="s">
         <v>64</v>
+      </c>
+      <c r="C8" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
generer fiche de poste
</commit_message>
<xml_diff>
--- a/tools/TODO.xlsx
+++ b/tools/TODO.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="114">
   <si>
     <t>créer des data de cv remplis</t>
   </si>
@@ -2056,10 +2056,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2232,7 +2232,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>103</v>
       </c>
@@ -2240,15 +2240,18 @@
         <v>63</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>111</v>
       </c>
       <c r="B18" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="C18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>104</v>
       </c>
@@ -2256,7 +2259,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>105</v>
       </c>
@@ -2264,7 +2267,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>106</v>
       </c>
@@ -2272,7 +2275,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>108</v>
       </c>
@@ -2280,7 +2283,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>109</v>
       </c>
@@ -2288,19 +2291,27 @@
         <v>113</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="B24" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>110</v>
+      </c>
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
         <v>107</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>